<commit_message>
Input LEDs and resistors added
</commit_message>
<xml_diff>
--- a/Logic/Logic_BOM.xlsx
+++ b/Logic/Logic_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kateartz/Desktop/OAM/Logic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F716A72-6F75-3547-964A-1DA48F3526D4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771589EB-74B3-C247-8416-687227DC281D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="2300" windowWidth="21660" windowHeight="13280" xr2:uid="{B76ABA8B-3CCB-C44F-8120-64FE1293F027}"/>
+    <workbookView xWindow="3500" yWindow="1800" windowWidth="21660" windowHeight="13280" xr2:uid="{B76ABA8B-3CCB-C44F-8120-64FE1293F027}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="87">
   <si>
     <t xml:space="preserve">Item # </t>
   </si>
@@ -57,18 +57,12 @@
     <t>R11,R14,R7,R9</t>
   </si>
   <si>
-    <t>R10,R12,R8,R13</t>
-  </si>
-  <si>
     <t>S6,S8,S5,S1,S7,S3,S2,S4</t>
   </si>
   <si>
     <t>Q3,Q2,Q1</t>
   </si>
   <si>
-    <t>D4,D2,D1,D3</t>
-  </si>
-  <si>
     <t>J3,J1,J6,J4,J7,J5,J2</t>
   </si>
   <si>
@@ -195,15 +189,6 @@
     <t>100 kOhms ±1% 0.1W, 1/10W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200 Thick Film</t>
   </si>
   <si>
-    <t>MC74ACT05DG</t>
-  </si>
-  <si>
-    <t>Onsemi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inverters 5V CMOS Hex w/Open Drain </t>
-  </si>
-  <si>
     <t xml:space="preserve">SOIC-14 </t>
   </si>
   <si>
@@ -289,6 +274,18 @@
   </si>
   <si>
     <t>10POS</t>
+  </si>
+  <si>
+    <t>SN74HCS125QBQARQ1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automotive Schmitt-trigger inputs quadruple bus buffer gates with 3-state outputs 14-WQFN -40 to 125 </t>
+  </si>
+  <si>
+    <t>D4,D2,D1,D3,D5,D6,D7</t>
+  </si>
+  <si>
+    <t>R10,R12,R8,R13,R15,R16,R17</t>
   </si>
 </sst>
 </file>
@@ -648,16 +645,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF8BDB-6D6C-F64B-95C4-377854EB9474}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="27.83203125" customWidth="1"/>
-    <col min="6" max="6" width="79" customWidth="1"/>
+    <col min="6" max="6" width="85.5" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="22.5" customWidth="1"/>
   </cols>
@@ -688,7 +685,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -702,16 +699,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -719,25 +716,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1">
         <v>1608</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -751,19 +748,19 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
         <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
       </c>
       <c r="G4" s="1">
         <v>1608</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -771,28 +768,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -800,25 +797,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -826,25 +823,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
         <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
       </c>
       <c r="G7" s="1">
         <v>3224</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -852,28 +849,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
         <v>44</v>
       </c>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -881,25 +878,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="1">
         <v>1005</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -907,22 +904,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -930,25 +927,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G11" s="1">
         <v>1005</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -956,25 +953,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -982,25 +979,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1008,25 +1005,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1034,28 +1031,28 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I15" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1063,25 +1060,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1089,22 +1086,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1112,25 +1109,25 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1138,19 +1135,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>